<commit_message>
add counter to stage 9 fixed comment and flow diagram
</commit_message>
<xml_diff>
--- a/flow diagram.xlsx
+++ b/flow diagram.xlsx
@@ -34,15 +34,9 @@
     <t>set z=0 and set x=9</t>
   </si>
   <si>
-    <t>set z=8.6</t>
-  </si>
-  <si>
     <t>grab off</t>
   </si>
   <si>
-    <t>base conveyor 1,2 on til part leaving</t>
-  </si>
-  <si>
     <t>start + stop blade 1 and stop blade 2 on</t>
   </si>
   <si>
@@ -68,6 +62,12 @@
   </si>
   <si>
     <t>stop blade2 off and set x=1.2 and set z=0.0</t>
+  </si>
+  <si>
+    <t>set z=8.4</t>
+  </si>
+  <si>
+    <t>base conveyor 1,2 on til part leaving and stop blade 2 on and counter +1</t>
   </si>
 </sst>
 </file>
@@ -1049,13 +1049,13 @@
   <dimension ref="J1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="52.7109375" customWidth="1"/>
-    <col min="12" max="12" width="73.5703125" customWidth="1"/>
+    <col min="12" max="12" width="92.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>1</v>
@@ -1090,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>2</v>
@@ -1104,7 +1104,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>4</v>
@@ -1118,7 +1118,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>3</v>
@@ -1146,10 +1146,10 @@
         <v>6</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1160,10 +1160,10 @@
         <v>7</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1174,10 +1174,10 @@
         <v>8</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1188,10 +1188,10 @@
         <v>9</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.25">

</xml_diff>